<commit_message>
add scene dragon points
增加场景龙的生成点；
增加采集物的生成点。
</commit_message>
<xml_diff>
--- a/Excels/CollectibleItem_采集物品表.xlsx
+++ b/Excels/CollectibleItem_采集物品表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E759AA7-A84F-4CCD-A2D8-42075245941C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A94F48-8EC9-4133-B596-22FFDFAB0EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,6 +148,97 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <color theme="1"/>
@@ -174,13 +265,6 @@
         <b/>
         <color theme="1"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79995117038483843"/>
@@ -197,86 +281,56 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79995117038483843"/>
           <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79995117038483843"/>
           <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
       <border>
         <left/>
         <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
+        <top style="double">
           <color theme="4"/>
         </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
+        <b/>
+        <color theme="0"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -302,82 +356,28 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <left/>
-        <right/>
-        <top style="double">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="11"/>
-      <tableStyleElement type="firstColumn" dxfId="16"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
       <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="0"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="6"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="1"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
       <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="4"/>
-      <tableStyleElement type="pageFieldValues" dxfId="3"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
+      <tableStyleElement type="pageFieldValues" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -601,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -713,17 +713,17 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0</v>
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4">
         <v>3600</v>
@@ -735,21 +735,21 @@
         <v>80</v>
       </c>
       <c r="H5" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
         <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
       </c>
       <c r="D6" s="4">
         <v>20</v>
@@ -758,7 +758,7 @@
         <v>3600</v>
       </c>
       <c r="F6" s="6">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="G6" s="1">
         <v>80</v>
@@ -772,10 +772,10 @@
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -787,7 +787,7 @@
         <v>3600</v>
       </c>
       <c r="F7" s="6">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="G7" s="1">
         <v>80</v>
@@ -796,41 +796,17 @@
         <v>5</v>
       </c>
       <c r="I7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="4">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4">
-        <v>3600</v>
-      </c>
-      <c r="F8" s="6">
-        <v>5</v>
-      </c>
-      <c r="G8" s="1">
-        <v>80</v>
-      </c>
-      <c r="H8" s="1">
-        <v>5</v>
-      </c>
-      <c r="I8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="6"/>
+    </row>
     <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="5"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
@@ -841,17 +817,24 @@
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="5"/>
-      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -859,6 +842,7 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="5"/>
@@ -901,7 +885,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="4"/>
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -910,11 +894,13 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -939,18 +925,8 @@
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
     </row>
     <row r="21" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
@@ -974,6 +950,7 @@
     </row>
     <row r="25" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
+      <c r="B25" s="5"/>
       <c r="D25" s="4"/>
       <c r="F25" s="6"/>
     </row>
@@ -985,7 +962,6 @@
     </row>
     <row r="27" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
-      <c r="B27" s="5"/>
       <c r="D27" s="4"/>
       <c r="F27" s="6"/>
     </row>
@@ -1027,7 +1003,6 @@
     <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="D35" s="4"/>
-      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
@@ -1035,7 +1010,7 @@
     </row>
     <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
-      <c r="D37" s="4"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
@@ -1061,11 +1036,7 @@
       <c r="A43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
-      <c r="D44" s="6"/>
-    </row>
-    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.0249999999999997" bottom="1.0249999999999997" header="0.78750000000000009" footer="0.78750000000000009"/>

</xml_diff>